<commit_message>
its been a while
</commit_message>
<xml_diff>
--- a/results/spreadsheets/All the possible investigatios to run.xlsx
+++ b/results/spreadsheets/All the possible investigatios to run.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9804"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="64">
   <si>
     <t>Broad Method</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>8gb not enough,5h</t>
-  </si>
-  <si>
-    <t>n</t>
   </si>
   <si>
     <t>16gb ne</t>
@@ -376,9 +373,7 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -394,7 +389,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,19 +674,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40:J40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -707,7 +704,7 @@
       <c r="I3" s="19"/>
       <c r="J3" s="19"/>
     </row>
-    <row r="4" spans="1:15" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="16"/>
       <c r="B4" s="18"/>
       <c r="C4" s="7" t="s">
@@ -744,28 +741,28 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
       <c r="K5" s="5"/>
       <c r="L5" s="6"/>
       <c r="M5" s="5"/>
       <c r="N5" s="6"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -797,7 +794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -829,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -861,7 +858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -893,28 +890,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
       <c r="K10" s="5"/>
       <c r="L10" s="6"/>
       <c r="M10" s="5"/>
       <c r="N10" s="6"/>
       <c r="O10" s="4"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="11" t="s">
         <v>42</v>
@@ -949,7 +946,7 @@
         <v>0.441299282969905</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" t="s">
         <v>27</v>
@@ -972,11 +969,11 @@
       <c r="L12" t="s">
         <v>56</v>
       </c>
-      <c r="O12" s="20">
+      <c r="O12" s="14">
         <v>0.77392382176012897</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" t="s">
         <v>28</v>
@@ -999,11 +996,11 @@
       <c r="L13" t="s">
         <v>55</v>
       </c>
-      <c r="O13" s="20">
+      <c r="O13" s="14">
         <v>0.38473473218037801</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" t="s">
         <v>29</v>
@@ -1026,11 +1023,11 @@
       <c r="L14" t="s">
         <v>57</v>
       </c>
-      <c r="O14" s="20">
+      <c r="O14" s="14">
         <v>0.303049984509838</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
         <v>30</v>
@@ -1063,7 +1060,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="10" t="s">
         <v>31</v>
@@ -1100,28 +1097,28 @@
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
     </row>
-    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
       <c r="K17" s="5"/>
       <c r="L17" s="6"/>
       <c r="M17" s="5"/>
       <c r="N17" s="6"/>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
@@ -1148,7 +1145,7 @@
       <c r="N18" s="13"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
@@ -1171,7 +1168,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
@@ -1194,7 +1191,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>32</v>
       </c>
@@ -1217,7 +1214,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>32</v>
       </c>
@@ -1240,7 +1237,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -1271,7 +1268,7 @@
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
         <v>42</v>
@@ -1294,7 +1291,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>33</v>
       </c>
@@ -1317,7 +1314,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
@@ -1340,7 +1337,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
@@ -1363,7 +1360,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
@@ -1386,7 +1383,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
@@ -1409,50 +1406,50 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
       <c r="K30" s="5"/>
       <c r="L30" s="6"/>
       <c r="M30" s="5"/>
       <c r="N30" s="6"/>
       <c r="O30" s="4"/>
     </row>
-    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
       <c r="K32" s="5"/>
       <c r="L32" s="6"/>
       <c r="M32" s="5"/>
       <c r="N32" s="6"/>
       <c r="O32" s="4"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1491,7 +1488,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -1529,28 +1526,28 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
       <c r="K35" s="5"/>
       <c r="L35" s="6"/>
       <c r="M35" s="5"/>
       <c r="N35" s="6"/>
       <c r="O35" s="4"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>44</v>
       </c>
@@ -1567,7 +1564,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>45</v>
       </c>
@@ -1578,7 +1575,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
@@ -1589,7 +1586,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>47</v>
       </c>
@@ -1600,30 +1597,30 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
       <c r="K40" s="5"/>
       <c r="L40" s="6"/>
       <c r="M40" s="5"/>
       <c r="N40" s="6"/>
       <c r="O40" s="4"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K41" t="s">
         <v>41</v>
@@ -1632,7 +1629,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>44</v>
       </c>
@@ -1640,10 +1637,10 @@
         <v>41</v>
       </c>
       <c r="L42" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>45</v>
       </c>
@@ -1651,10 +1648,10 @@
         <v>41</v>
       </c>
       <c r="L43" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>30</v>
       </c>
@@ -1662,13 +1659,13 @@
         <v>41</v>
       </c>
       <c r="L44" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="M44" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>31</v>
       </c>
@@ -1676,29 +1673,29 @@
         <v>41</v>
       </c>
       <c r="L45" t="s">
+        <v>35</v>
+      </c>
+      <c r="M45" t="s">
         <v>61</v>
       </c>
-      <c r="M45" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>44</v>
       </c>
@@ -1709,7 +1706,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>45</v>
       </c>
@@ -1720,7 +1717,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>30</v>
       </c>
@@ -1731,7 +1728,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>31</v>
       </c>
@@ -1744,17 +1741,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B17:J17"/>
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B46:J46"/>
     <mergeCell ref="B35:J35"/>
     <mergeCell ref="B30:J30"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B32:J32"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B17:J17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>